<commit_message>
merge with random planar graph
</commit_message>
<xml_diff>
--- a/adjacent data -- ff.xlsx
+++ b/adjacent data -- ff.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>G</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -468,12 +468,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -483,12 +483,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>M</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -498,12 +498,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>H</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -513,12 +513,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -528,12 +528,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>K</t>
+          <t>S</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -543,12 +543,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>F</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>H</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -558,12 +558,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>J</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Q</t>
+          <t>L</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -573,12 +573,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>O</t>
+          <t>I</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -588,12 +588,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>L</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -603,12 +603,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>K</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -618,12 +618,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>R</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -638,7 +638,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>P</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -648,12 +648,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>H</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>Q</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -663,12 +663,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>G</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>O</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -678,7 +678,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -693,12 +693,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>G</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -708,12 +708,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -723,12 +723,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>S</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>C</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -738,12 +738,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>E</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -753,12 +753,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>L</t>
+          <t>N</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -768,7 +768,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>L</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -783,7 +783,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -798,12 +798,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>J</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>J</t>
+          <t>M</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -813,15 +813,30 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>K</t>
         </is>
       </c>
       <c r="C26" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>